<commit_message>
Buggy code with swtich statements
</commit_message>
<xml_diff>
--- a/LexicalAnalyzer/ExcelSymbolTable.xlsx
+++ b/LexicalAnalyzer/ExcelSymbolTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="25">
   <si>
     <t xml:space="preserve">L</t>
   </si>
@@ -40,6 +40,27 @@
     <t xml:space="preserve">&lt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">)</t>
+  </si>
+  <si>
     <t xml:space="preserve">space</t>
   </si>
   <si>
@@ -62,6 +83,18 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;relop&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;comma&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;semi&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;bracket&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;parenth&gt;</t>
   </si>
 </sst>
 </file>
@@ -135,12 +168,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,10 +304,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N27" activeCellId="0" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -300,6 +337,27 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -321,9 +379,32 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="O2" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -347,31 +428,73 @@
       <c r="G3" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -395,31 +518,73 @@
       <c r="G5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -443,31 +608,73 @@
       <c r="G7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -491,7 +698,28 @@
       <c r="G9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -515,7 +743,28 @@
       <c r="G10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -539,31 +788,73 @@
       <c r="G11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -587,55 +878,118 @@
       <c r="G13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -659,65 +1013,515 @@
       <c r="G16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="O16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="A19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
1st FSA passed. Token list generated.
</commit_message>
<xml_diff>
--- a/LexicalAnalyzer/ExcelSymbolTable.xlsx
+++ b/LexicalAnalyzer/ExcelSymbolTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="29">
   <si>
     <t xml:space="preserve">L</t>
   </si>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">)</t>
   </si>
   <si>
+    <t xml:space="preserve">plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minus</t>
+  </si>
+  <si>
     <t xml:space="preserve">space</t>
   </si>
   <si>
@@ -95,6 +101,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;parenth&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;addop&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;minop&gt;</t>
   </si>
 </sst>
 </file>
@@ -109,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -168,7 +181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,8 +190,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -304,10 +321,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N27" activeCellId="0" sqref="N27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -358,6 +375,12 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -400,9 +423,15 @@
         <v>25</v>
       </c>
       <c r="N2" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="Q2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -449,52 +478,64 @@
       <c r="N3" s="1" t="n">
         <v>-1</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="O3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -539,52 +580,64 @@
       <c r="N5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="O5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -629,52 +682,64 @@
       <c r="N7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="O7" s="1"/>
+      <c r="O7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -719,7 +784,13 @@
       <c r="N9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="O9" s="1"/>
+      <c r="O9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="P9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -764,7 +835,13 @@
       <c r="N10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="O10" s="1"/>
+      <c r="O10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="P10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -809,52 +886,64 @@
       <c r="N11" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="O11" s="1"/>
+      <c r="O11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -899,97 +988,115 @@
       <c r="N13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="O13" s="1"/>
+      <c r="O13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O15" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1034,97 +1141,115 @@
       <c r="N16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="O16" s="1"/>
+      <c r="O16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O18" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -1169,358 +1294,512 @@
       <c r="N19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="O19" s="1"/>
+      <c r="O19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>20</v>
+      <c r="A21" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22" s="0" t="s">
-        <v>21</v>
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="N23" s="0" t="s">
-        <v>22</v>
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N24" s="0" t="s">
-        <v>23</v>
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="N25" s="0" t="s">
-        <v>23</v>
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="N26" s="0" t="s">
-        <v>24</v>
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="N27" s="0" t="s">
-        <v>24</v>
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>